<commit_message>
bugfix chemical import and template table
</commit_message>
<xml_diff>
--- a/rotmic/static/uploadexample_chemicalcomponent.xlsx
+++ b/rotmic/static/uploadexample_chemicalcomponent.xlsx
@@ -60,9 +60,6 @@
     <t>ordered</t>
   </si>
   <si>
-    <t>hypothetical</t>
-  </si>
-  <si>
     <t>Import of Oligonucleotides</t>
   </si>
   <si>
@@ -102,10 +99,13 @@
     <t>reagent / solvents</t>
   </si>
   <si>
-    <t>mtchem001</t>
-  </si>
-  <si>
-    <t>EtOH</t>
+    <t>mtchem0002</t>
+  </si>
+  <si>
+    <t>MetOH</t>
+  </si>
+  <si>
+    <t>Methanol p.a.</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -514,7 +514,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -536,7 +536,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>4</v>
@@ -544,22 +544,22 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -567,7 +567,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="10"/>
     </row>
@@ -576,7 +576,7 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="10"/>
     </row>
@@ -585,7 +585,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="10"/>
     </row>
@@ -594,7 +594,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" s="10"/>
     </row>
@@ -603,7 +603,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" s="10"/>
     </row>
@@ -612,7 +612,7 @@
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" s="10"/>
     </row>
@@ -621,7 +621,7 @@
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="10"/>
     </row>
@@ -630,7 +630,7 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" s="10"/>
     </row>
@@ -639,7 +639,7 @@
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" s="10"/>
     </row>
@@ -648,7 +648,7 @@
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="10"/>
     </row>
@@ -657,7 +657,7 @@
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" s="10"/>
     </row>
@@ -666,7 +666,7 @@
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17" s="10"/>
     </row>
@@ -675,7 +675,7 @@
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" s="10"/>
     </row>
@@ -684,7 +684,7 @@
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="10"/>
     </row>
@@ -693,7 +693,7 @@
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E20" s="10"/>
     </row>
@@ -702,7 +702,7 @@
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E21" s="10"/>
     </row>
@@ -711,7 +711,7 @@
         <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E22" s="10"/>
     </row>
@@ -720,7 +720,7 @@
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E23" s="10"/>
     </row>
@@ -729,7 +729,7 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E24" s="10"/>
     </row>
@@ -738,7 +738,7 @@
         <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E25" s="10"/>
     </row>
@@ -747,7 +747,7 @@
         <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E26" s="10"/>
     </row>
@@ -756,7 +756,7 @@
         <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E27" s="10"/>
     </row>
@@ -765,7 +765,7 @@
         <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E28" s="10"/>
     </row>
@@ -774,7 +774,7 @@
         <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E29" s="10"/>
     </row>
@@ -783,7 +783,7 @@
         <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E30" s="10"/>
     </row>
@@ -792,7 +792,7 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E31" s="10"/>
     </row>
@@ -801,7 +801,7 @@
         <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E32" s="10"/>
     </row>
@@ -810,7 +810,7 @@
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E33" s="10"/>
     </row>
@@ -819,7 +819,7 @@
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E34" s="10"/>
     </row>
@@ -828,7 +828,7 @@
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E35" s="10"/>
     </row>
@@ -837,7 +837,7 @@
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E36" s="10"/>
     </row>
@@ -846,7 +846,7 @@
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E37" s="10"/>
     </row>
@@ -855,7 +855,7 @@
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E38" s="10"/>
     </row>
@@ -864,7 +864,7 @@
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E39" s="10"/>
     </row>
@@ -873,7 +873,7 @@
         <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E40" s="10"/>
     </row>
@@ -882,7 +882,7 @@
         <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E41" s="10"/>
     </row>
@@ -891,7 +891,7 @@
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E42" s="10"/>
     </row>
@@ -951,7 +951,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L5" t="s">
         <v>10</v>
@@ -962,7 +962,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L6" t="s">
         <v>10</v>
@@ -973,7 +973,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L7" t="s">
         <v>10</v>
@@ -984,7 +984,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L8" t="s">
         <v>10</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L9" t="s">
         <v>10</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L10" t="s">
         <v>10</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L11" t="s">
         <v>10</v>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L12" t="s">
         <v>10</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L13" t="s">
         <v>10</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L14" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
proteincomponent / sample upload
</commit_message>
<xml_diff>
--- a/rotmic/static/uploadexample_chemicalcomponent.xlsx
+++ b/rotmic/static/uploadexample_chemicalcomponent.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="75" windowWidth="26265" windowHeight="15390"/>
+    <workbookView xWindow="45" yWindow="75" windowWidth="25440" windowHeight="15390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>ordered</t>
   </si>
   <si>
-    <t>Import of Oligonucleotides</t>
-  </si>
-  <si>
     <t>C.A.S.</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>Methanol p.a.</t>
+  </si>
+  <si>
+    <t>Import of Chemicals &amp; Reagents</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -514,7 +514,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -536,7 +536,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>4</v>
@@ -544,22 +544,22 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -567,7 +567,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="10"/>
     </row>
@@ -576,7 +576,7 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="10"/>
     </row>
@@ -585,7 +585,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="10"/>
     </row>
@@ -594,7 +594,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="10"/>
     </row>
@@ -603,7 +603,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" s="10"/>
     </row>
@@ -612,7 +612,7 @@
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" s="10"/>
     </row>
@@ -621,7 +621,7 @@
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" s="10"/>
     </row>
@@ -630,7 +630,7 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" s="10"/>
     </row>
@@ -639,7 +639,7 @@
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="10"/>
     </row>
@@ -648,7 +648,7 @@
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" s="10"/>
     </row>
@@ -657,7 +657,7 @@
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" s="10"/>
     </row>
@@ -666,7 +666,7 @@
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17" s="10"/>
     </row>
@@ -675,7 +675,7 @@
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" s="10"/>
     </row>
@@ -684,7 +684,7 @@
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" s="10"/>
     </row>
@@ -693,7 +693,7 @@
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E20" s="10"/>
     </row>
@@ -702,7 +702,7 @@
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21" s="10"/>
     </row>
@@ -711,7 +711,7 @@
         <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E22" s="10"/>
     </row>
@@ -720,7 +720,7 @@
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E23" s="10"/>
     </row>
@@ -729,7 +729,7 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E24" s="10"/>
     </row>
@@ -738,7 +738,7 @@
         <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E25" s="10"/>
     </row>
@@ -747,7 +747,7 @@
         <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E26" s="10"/>
     </row>
@@ -756,7 +756,7 @@
         <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E27" s="10"/>
     </row>
@@ -765,7 +765,7 @@
         <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E28" s="10"/>
     </row>
@@ -774,7 +774,7 @@
         <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E29" s="10"/>
     </row>
@@ -783,7 +783,7 @@
         <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E30" s="10"/>
     </row>
@@ -792,7 +792,7 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E31" s="10"/>
     </row>
@@ -801,7 +801,7 @@
         <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E32" s="10"/>
     </row>
@@ -810,7 +810,7 @@
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E33" s="10"/>
     </row>
@@ -819,7 +819,7 @@
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E34" s="10"/>
     </row>
@@ -828,7 +828,7 @@
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E35" s="10"/>
     </row>
@@ -837,7 +837,7 @@
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E36" s="10"/>
     </row>
@@ -846,7 +846,7 @@
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E37" s="10"/>
     </row>
@@ -855,7 +855,7 @@
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E38" s="10"/>
     </row>
@@ -864,7 +864,7 @@
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E39" s="10"/>
     </row>
@@ -873,7 +873,7 @@
         <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E40" s="10"/>
     </row>
@@ -882,7 +882,7 @@
         <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E41" s="10"/>
     </row>
@@ -891,7 +891,7 @@
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E42" s="10"/>
     </row>
@@ -951,7 +951,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L5" t="s">
         <v>10</v>
@@ -962,7 +962,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L6" t="s">
         <v>10</v>
@@ -973,7 +973,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L7" t="s">
         <v>10</v>
@@ -984,7 +984,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L8" t="s">
         <v>10</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L9" t="s">
         <v>10</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L10" t="s">
         <v>10</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L11" t="s">
         <v>10</v>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="C12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L12" t="s">
         <v>10</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L13" t="s">
         <v>10</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L14" t="s">
         <v>10</v>

</xml_diff>